<commit_message>
Update Excel template with additional fields for Azure storage
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0a650c88-9d3d-45f7-af58-a2cd5dec0be5
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/99e565d9-defe-4b43-9370-4d17ce50e7be/a555d384-6dbf-49ef-8148-16450a44e72d.jpg
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -425,6 +425,7 @@
     <col min="21" max="21" width="20.83203125" customWidth="1"/>
     <col min="22" max="22" width="15.83203125" customWidth="1"/>
     <col min="23" max="23" width="15.83203125" customWidth="1"/>
+    <col min="24" max="24" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -441,34 +442,34 @@
         <v>call_date</v>
       </c>
       <c r="E1" t="str">
-        <v>auditRole</v>
+        <v>Audit Role</v>
       </c>
       <c r="F1" t="str">
-        <v>OLMSID</v>
+        <v>AgentID</v>
       </c>
       <c r="G1" t="str">
-        <v>Name</v>
+        <v>AgentName</v>
       </c>
       <c r="H1" t="str">
-        <v>PBXID</v>
+        <v>PBX ID</v>
       </c>
       <c r="I1" t="str">
-        <v>partnerName</v>
+        <v>Partner Name</v>
       </c>
       <c r="J1" t="str">
-        <v>customerMobile</v>
+        <v>Customer Mobile</v>
       </c>
       <c r="K1" t="str">
-        <v>callDuration</v>
+        <v>Call Duration</v>
       </c>
       <c r="L1" t="str">
-        <v>callType</v>
+        <v>Call Type</v>
       </c>
       <c r="M1" t="str">
-        <v>subType</v>
+        <v>Sub Type</v>
       </c>
       <c r="N1" t="str">
-        <v>subSubType</v>
+        <v>Sub sub Type</v>
       </c>
       <c r="O1" t="str">
         <v>VOC</v>
@@ -480,7 +481,7 @@
         <v>userRole</v>
       </c>
       <c r="R1" t="str">
-        <v>advisorCategory</v>
+        <v>Advisor Category</v>
       </c>
       <c r="S1" t="str">
         <v>businessSegment</v>
@@ -492,9 +493,12 @@
         <v>formName</v>
       </c>
       <c r="V1" t="str">
+        <v>Campaign</v>
+      </c>
+      <c r="W1" t="str">
         <v>callId</v>
       </c>
-      <c r="W1" t="str">
+      <c r="X1" t="str">
         <v>callDate</v>
       </c>
     </row>
@@ -563,15 +567,18 @@
         <v>Evaluation Form 1</v>
       </c>
       <c r="V2" t="str">
+        <v>Spring Promo 2025</v>
+      </c>
+      <c r="W2" t="str">
         <v>CALL-123-25</v>
       </c>
-      <c r="W2" t="str">
+      <c r="X2" t="str">
         <v>2025-04-03</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:W2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>